<commit_message>
1ra modificacion en master BORRADOR1
</commit_message>
<xml_diff>
--- a/CRONOGRAMA.xlsx
+++ b/CRONOGRAMA.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\2021\UdeA\S3 2023-1\INFO II\TEORIA\_REPOSITORIO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AndresRivera\REPOSITORIO\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="23">
   <si>
     <t>FEBRERO</t>
   </si>
@@ -90,12 +90,15 @@
   </si>
   <si>
     <t>Informática II</t>
+  </si>
+  <si>
+    <t>BORRADOR1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -590,7 +593,7 @@
   <dimension ref="A1:AN42"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1690,7 +1693,9 @@
       <c r="AN23" s="12"/>
     </row>
     <row r="24" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A24" s="8"/>
+      <c r="A24" s="8" t="s">
+        <v>22</v>
+      </c>
       <c r="B24" s="14"/>
       <c r="C24" s="17">
         <v>0.91666666666666696</v>

</xml_diff>